<commit_message>
Update Qogita Analyse v3_check+JEWLWW(photo).xlsx
</commit_message>
<xml_diff>
--- a/Qogita Analyse v3_check+JEWLWW(photo).xlsx
+++ b/Qogita Analyse v3_check+JEWLWW(photo).xlsx
@@ -865,7 +865,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr"/>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S4" t="inlineStr">
         <is>
           <t>48k (1%)</t>
@@ -973,7 +977,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr"/>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="S5" t="inlineStr">
         <is>
           <t>51k (1%)</t>
@@ -1077,7 +1085,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr"/>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="S6" t="inlineStr">
         <is>
           <t>175k (3%)</t>
@@ -1181,7 +1193,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr"/>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S7" t="inlineStr">
         <is>
           <t>64k (2%)</t>
@@ -1285,7 +1301,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr"/>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="S8" t="inlineStr">
         <is>
           <t>89k (2%)</t>
@@ -1389,7 +1409,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr"/>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S9" t="inlineStr">
         <is>
           <t>71k (2%)</t>
@@ -1493,7 +1517,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S10" t="inlineStr">
         <is>
           <t>21k (1%)</t>
@@ -1597,7 +1625,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S11" t="inlineStr">
         <is>
           <t>52k (1%)</t>
@@ -1701,7 +1733,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S12" t="inlineStr">
         <is>
           <t>98k (2%)</t>
@@ -1805,7 +1841,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr"/>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S13" t="inlineStr">
         <is>
           <t>45k (1%)</t>
@@ -1909,7 +1949,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr"/>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S14" t="inlineStr">
         <is>
           <t>44k (1%)</t>
@@ -2021,7 +2065,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr"/>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S15" t="inlineStr">
         <is>
           <t>34k (1%)</t>
@@ -2129,7 +2177,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S16" t="inlineStr">
         <is>
           <t>91k (2%)</t>
@@ -2233,7 +2285,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S17" t="inlineStr">
         <is>
           <t>90k (2%)</t>
@@ -2337,7 +2393,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="S18" t="inlineStr">
         <is>
           <t>67k (2%)</t>
@@ -2441,7 +2501,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S19" t="inlineStr">
         <is>
           <t>108k (2%)</t>
@@ -2545,7 +2609,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S20" t="inlineStr">
         <is>
           <t>113k (2%)</t>
@@ -2657,7 +2725,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr"/>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="S21" t="inlineStr">
         <is>
           <t>197k (4%)</t>
@@ -2761,7 +2833,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr"/>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S22" t="inlineStr">
         <is>
           <t>179k (3%)</t>
@@ -2863,7 +2939,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="S23" t="inlineStr">
         <is>
           <t>31k (1%)</t>
@@ -2967,7 +3047,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S24" t="inlineStr">
         <is>
           <t>335k (6%)</t>
@@ -3071,7 +3155,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="R25" t="inlineStr"/>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="S25" t="inlineStr">
         <is>
           <t>281k (1%)</t>

</xml_diff>